<commit_message>
8 models trained against hardoded
</commit_message>
<xml_diff>
--- a/data/g_vs_hardcoded_COIN_1_checkers.xlsx
+++ b/data/g_vs_hardcoded_COIN_1_checkers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -478,10 +478,75 @@
         </is>
       </c>
       <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
         <v>100</v>
       </c>
-      <c r="C4" t="n">
-        <v>20</v>
+      <c r="C5" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>100</v>
+      </c>
+      <c r="C7" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>100</v>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>100</v>
+      </c>
+      <c r="C9" t="n">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tested models against 1-checker hardcoded COIN, hoping to show some progress
</commit_message>
<xml_diff>
--- a/data/g_vs_hardcoded_COIN_1_checkers.xlsx
+++ b/data/g_vs_hardcoded_COIN_1_checkers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>22</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         <v>100</v>
       </c>
       <c r="C5" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C6" t="n">
-        <v>23</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
@@ -520,33 +520,397 @@
         <v>100</v>
       </c>
       <c r="C7" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>6</t>
+          <t>7</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>100</v>
       </c>
       <c r="C8" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>7</t>
+          <t>9</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>100</v>
+      </c>
+      <c r="C10" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>100</v>
+      </c>
+      <c r="C11" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>100</v>
+      </c>
+      <c r="C12" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>100</v>
+      </c>
+      <c r="C13" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>100</v>
+      </c>
+      <c r="C14" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>100</v>
+      </c>
+      <c r="C16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>25</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="inlineStr">
+        <is>
+          <t>27</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>100</v>
+      </c>
+      <c r="C18" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="inlineStr">
+        <is>
+          <t>29</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="inlineStr">
+        <is>
+          <t>31</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
+        <is>
+          <t>33</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>100</v>
+      </c>
+      <c r="C21" t="n">
         <v>9</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="inlineStr">
+        <is>
+          <t>35</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>100</v>
+      </c>
+      <c r="C22" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>100</v>
+      </c>
+      <c r="C23" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="inlineStr">
+        <is>
+          <t>39</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>100</v>
+      </c>
+      <c r="C24" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="inlineStr">
+        <is>
+          <t>41</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="inlineStr">
+        <is>
+          <t>43</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>100</v>
+      </c>
+      <c r="C26" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>100</v>
+      </c>
+      <c r="C27" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>46</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>100</v>
+      </c>
+      <c r="C28" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="inlineStr">
+        <is>
+          <t>47</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>100</v>
+      </c>
+      <c r="C29" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="inlineStr">
+        <is>
+          <t>48</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>0</v>
+      </c>
+      <c r="C30" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>49</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>100</v>
+      </c>
+      <c r="C31" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="inlineStr">
+        <is>
+          <t>51</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>100</v>
+      </c>
+      <c r="C33" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="inlineStr">
+        <is>
+          <t>52</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>100</v>
+      </c>
+      <c r="C34" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>53</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>100</v>
+      </c>
+      <c r="C35" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="inlineStr">
+        <is>
+          <t>54</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>100</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="inlineStr">
+        <is>
+          <t>55</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran updated hardcoded 1-checker test
</commit_message>
<xml_diff>
--- a/data/g_vs_hardcoded_COIN_1_checkers.xlsx
+++ b/data/g_vs_hardcoded_COIN_1_checkers.xlsx
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>33.7</v>
       </c>
       <c r="C2" t="n">
-        <v>33</v>
+        <v>13.236</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>100</v>
+        <v>83.5</v>
       </c>
       <c r="C3" t="n">
-        <v>4</v>
+        <v>4.983</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>22.338</v>
       </c>
     </row>
     <row r="5">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>66</v>
       </c>
       <c r="C5" t="n">
-        <v>5</v>
+        <v>5.173</v>
       </c>
     </row>
     <row r="6">
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>100</v>
+        <v>85.7</v>
       </c>
       <c r="C6" t="n">
-        <v>2</v>
+        <v>4.201</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>100</v>
       </c>
       <c r="C7" t="n">
-        <v>9</v>
+        <v>6.875</v>
       </c>
     </row>
     <row r="8">
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>100</v>
+        <v>82.3</v>
       </c>
       <c r="C8" t="n">
-        <v>11</v>
+        <v>9.23</v>
       </c>
     </row>
     <row r="9">
@@ -543,10 +543,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0</v>
+        <v>51.2</v>
       </c>
       <c r="C9" t="n">
-        <v>3</v>
+        <v>4.282</v>
       </c>
     </row>
     <row r="10">
@@ -585,7 +585,7 @@
         <v>100</v>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>8.872999999999999</v>
       </c>
     </row>
     <row r="13">
@@ -595,10 +595,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>100</v>
+        <v>33.1</v>
       </c>
       <c r="C13" t="n">
-        <v>24</v>
+        <v>22.808</v>
       </c>
     </row>
     <row r="14">
@@ -608,10 +608,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>100</v>
+        <v>51.2</v>
       </c>
       <c r="C14" t="n">
-        <v>21</v>
+        <v>26.856</v>
       </c>
     </row>
     <row r="15">
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0</v>
+        <v>14.3</v>
       </c>
       <c r="C15" t="n">
-        <v>22</v>
+        <v>22.143</v>
       </c>
     </row>
     <row r="16">
@@ -634,10 +634,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>100</v>
+        <v>84.2</v>
       </c>
       <c r="C16" t="n">
-        <v>5</v>
+        <v>6.94</v>
       </c>
     </row>
     <row r="17">
@@ -647,10 +647,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0</v>
+        <v>32.4</v>
       </c>
       <c r="C17" t="n">
-        <v>3</v>
+        <v>8.964</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         <v>100</v>
       </c>
       <c r="C18" t="n">
-        <v>5</v>
+        <v>5.184</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>22</v>
+        <v>14.984</v>
       </c>
     </row>
     <row r="20">
@@ -702,7 +702,7 @@
         <v>100</v>
       </c>
       <c r="C21" t="n">
-        <v>9</v>
+        <v>13.716</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         <v>100</v>
       </c>
       <c r="C22" t="n">
-        <v>19</v>
+        <v>22.633</v>
       </c>
     </row>
     <row r="23">
@@ -767,7 +767,7 @@
         <v>100</v>
       </c>
       <c r="C26" t="n">
-        <v>15</v>
+        <v>15.814</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         <v>100</v>
       </c>
       <c r="C27" t="n">
-        <v>11</v>
+        <v>9.032</v>
       </c>
     </row>
     <row r="28">
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>100</v>
+        <v>81.09999999999999</v>
       </c>
       <c r="C28" t="n">
-        <v>11</v>
+        <v>5.291</v>
       </c>
     </row>
     <row r="29">
@@ -803,10 +803,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>100</v>
+        <v>65</v>
       </c>
       <c r="C29" t="n">
-        <v>3</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>21</v>
+        <v>16.443</v>
       </c>
     </row>
     <row r="31">
@@ -829,10 +829,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>100</v>
+        <v>18.5</v>
       </c>
       <c r="C31" t="n">
-        <v>3</v>
+        <v>27.45</v>
       </c>
     </row>
     <row r="32">
@@ -842,10 +842,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>0</v>
+        <v>50.6</v>
       </c>
       <c r="C32" t="n">
-        <v>2</v>
+        <v>8.375</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         <v>100</v>
       </c>
       <c r="C33" t="n">
-        <v>5</v>
+        <v>4.949</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         <v>100</v>
       </c>
       <c r="C34" t="n">
-        <v>5</v>
+        <v>4.673</v>
       </c>
     </row>
     <row r="35">
@@ -881,10 +881,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>100</v>
+        <v>83.40000000000001</v>
       </c>
       <c r="C35" t="n">
-        <v>22</v>
+        <v>16.556</v>
       </c>
     </row>
     <row r="36">
@@ -894,10 +894,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>100</v>
+        <v>47.3</v>
       </c>
       <c r="C36" t="n">
-        <v>4</v>
+        <v>3.657</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>21</v>
+        <v>17.98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Trained some g-models against 1 checker hardcoded
</commit_message>
<xml_diff>
--- a/data/g_vs_hardcoded_COIN_1_checkers.xlsx
+++ b/data/g_vs_hardcoded_COIN_1_checkers.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33.7</v>
+        <v>35</v>
       </c>
       <c r="C2" t="n">
-        <v>13.236</v>
+        <v>12.523</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>83.5</v>
+        <v>84.5</v>
       </c>
       <c r="C3" t="n">
-        <v>4.983</v>
+        <v>5.026</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>22.338</v>
+        <v>22.322</v>
       </c>
     </row>
     <row r="5">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>66</v>
+        <v>64.59999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>5.173</v>
+        <v>5.062</v>
       </c>
     </row>
     <row r="6">
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>85.7</v>
+        <v>84.59999999999999</v>
       </c>
       <c r="C6" t="n">
-        <v>4.201</v>
+        <v>4.185</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>100</v>
       </c>
       <c r="C7" t="n">
-        <v>6.875</v>
+        <v>7.07</v>
       </c>
     </row>
     <row r="8">
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>82.3</v>
+        <v>82.59999999999999</v>
       </c>
       <c r="C8" t="n">
-        <v>9.23</v>
+        <v>9.26</v>
       </c>
     </row>
     <row r="9">
@@ -543,10 +543,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>51.2</v>
+        <v>49.9</v>
       </c>
       <c r="C9" t="n">
-        <v>4.282</v>
+        <v>4.152</v>
       </c>
     </row>
     <row r="10">
@@ -585,7 +585,7 @@
         <v>100</v>
       </c>
       <c r="C12" t="n">
-        <v>8.872999999999999</v>
+        <v>8.701000000000001</v>
       </c>
     </row>
     <row r="13">
@@ -595,7 +595,7 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>33.1</v>
+        <v>31.7</v>
       </c>
       <c r="C13" t="n">
         <v>22.808</v>
@@ -608,10 +608,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>51.2</v>
+        <v>49</v>
       </c>
       <c r="C14" t="n">
-        <v>26.856</v>
+        <v>27.12</v>
       </c>
     </row>
     <row r="15">
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>14.3</v>
+        <v>18.6</v>
       </c>
       <c r="C15" t="n">
-        <v>22.143</v>
+        <v>22.186</v>
       </c>
     </row>
     <row r="16">
@@ -634,10 +634,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>84.2</v>
+        <v>82.59999999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>6.94</v>
+        <v>6.524</v>
       </c>
     </row>
     <row r="17">
@@ -647,10 +647,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>32.4</v>
+        <v>32.5</v>
       </c>
       <c r="C17" t="n">
-        <v>8.964</v>
+        <v>9.718</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         <v>100</v>
       </c>
       <c r="C18" t="n">
-        <v>5.184</v>
+        <v>5.16</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>14.984</v>
+        <v>14.858</v>
       </c>
     </row>
     <row r="20">
@@ -702,7 +702,7 @@
         <v>100</v>
       </c>
       <c r="C21" t="n">
-        <v>13.716</v>
+        <v>13.743</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         <v>100</v>
       </c>
       <c r="C22" t="n">
-        <v>22.633</v>
+        <v>22.262</v>
       </c>
     </row>
     <row r="23">
@@ -767,7 +767,7 @@
         <v>100</v>
       </c>
       <c r="C26" t="n">
-        <v>15.814</v>
+        <v>15.794</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         <v>100</v>
       </c>
       <c r="C27" t="n">
-        <v>9.032</v>
+        <v>8.968</v>
       </c>
     </row>
     <row r="28">
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>81.09999999999999</v>
+        <v>83.40000000000001</v>
       </c>
       <c r="C28" t="n">
-        <v>5.291</v>
+        <v>5.781</v>
       </c>
     </row>
     <row r="29">
@@ -803,10 +803,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>65</v>
+        <v>68.2</v>
       </c>
       <c r="C29" t="n">
-        <v>3.9</v>
+        <v>4.046</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>16.443</v>
+        <v>15.999</v>
       </c>
     </row>
     <row r="31">
@@ -829,10 +829,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>18.5</v>
+        <v>18.1</v>
       </c>
       <c r="C31" t="n">
-        <v>27.45</v>
+        <v>27.57</v>
       </c>
     </row>
     <row r="32">
@@ -842,10 +842,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>50.6</v>
+        <v>50</v>
       </c>
       <c r="C32" t="n">
-        <v>8.375</v>
+        <v>7.979</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         <v>100</v>
       </c>
       <c r="C33" t="n">
-        <v>4.949</v>
+        <v>4.934</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         <v>100</v>
       </c>
       <c r="C34" t="n">
-        <v>4.673</v>
+        <v>4.646</v>
       </c>
     </row>
     <row r="35">
@@ -881,10 +881,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>83.40000000000001</v>
+        <v>84</v>
       </c>
       <c r="C35" t="n">
-        <v>16.556</v>
+        <v>17.561</v>
       </c>
     </row>
     <row r="36">
@@ -894,10 +894,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>47.3</v>
+        <v>48.5</v>
       </c>
       <c r="C36" t="n">
-        <v>3.657</v>
+        <v>3.666</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,137 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>17.98</v>
+        <v>17.68</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="inlineStr">
+        <is>
+          <t>56</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>84.5</v>
+      </c>
+      <c r="C38" t="n">
+        <v>7.438</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>57</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>100</v>
+      </c>
+      <c r="C39" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="inlineStr">
+        <is>
+          <t>58</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>49.5</v>
+      </c>
+      <c r="C40" t="n">
+        <v>8.489000000000001</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="inlineStr">
+        <is>
+          <t>59</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>100</v>
+      </c>
+      <c r="C41" t="n">
+        <v>4.958</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="inlineStr">
+        <is>
+          <t>60</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>50.2</v>
+      </c>
+      <c r="C42" t="n">
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr">
+        <is>
+          <t>61</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>100</v>
+      </c>
+      <c r="C43" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="inlineStr">
+        <is>
+          <t>62</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>100</v>
+      </c>
+      <c r="C44" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>63</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>17.5</v>
+      </c>
+      <c r="C45" t="n">
+        <v>13.554</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>64</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>49.9</v>
+      </c>
+      <c r="C46" t="n">
+        <v>19.051</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>16.3</v>
+      </c>
+      <c r="C47" t="n">
+        <v>4.52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran a few more tests
</commit_message>
<xml_diff>
--- a/data/g_vs_hardcoded_COIN_1_checkers.xlsx
+++ b/data/g_vs_hardcoded_COIN_1_checkers.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="guerrilla vs. hardcoded COIN 1 checkers" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="g vs. hardcoded C 1 checkers" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -452,10 +452,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" t="n">
-        <v>12.523</v>
+        <v>12.821</v>
       </c>
     </row>
     <row r="3">
@@ -465,10 +465,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>84.5</v>
+        <v>82</v>
       </c>
       <c r="C3" t="n">
-        <v>5.026</v>
+        <v>4.965</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         <v>0</v>
       </c>
       <c r="C4" t="n">
-        <v>22.322</v>
+        <v>22.352</v>
       </c>
     </row>
     <row r="5">
@@ -491,10 +491,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>64.59999999999999</v>
+        <v>67.09999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>5.062</v>
+        <v>5.227</v>
       </c>
     </row>
     <row r="6">
@@ -504,10 +504,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>84.59999999999999</v>
+        <v>84.7</v>
       </c>
       <c r="C6" t="n">
-        <v>4.185</v>
+        <v>4.205</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         <v>100</v>
       </c>
       <c r="C7" t="n">
-        <v>7.07</v>
+        <v>7.013</v>
       </c>
     </row>
     <row r="8">
@@ -530,10 +530,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>82.59999999999999</v>
+        <v>85.3</v>
       </c>
       <c r="C8" t="n">
-        <v>9.26</v>
+        <v>9.529999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -543,10 +543,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>49.9</v>
+        <v>48.6</v>
       </c>
       <c r="C9" t="n">
-        <v>4.152</v>
+        <v>4.011</v>
       </c>
     </row>
     <row r="10">
@@ -585,7 +585,7 @@
         <v>100</v>
       </c>
       <c r="C12" t="n">
-        <v>8.701000000000001</v>
+        <v>8.801</v>
       </c>
     </row>
     <row r="13">
@@ -595,10 +595,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>31.7</v>
+        <v>31.9</v>
       </c>
       <c r="C13" t="n">
-        <v>22.808</v>
+        <v>22.788</v>
       </c>
     </row>
     <row r="14">
@@ -608,10 +608,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>49</v>
+        <v>52.1</v>
       </c>
       <c r="C14" t="n">
-        <v>27.12</v>
+        <v>26.748</v>
       </c>
     </row>
     <row r="15">
@@ -621,10 +621,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>18.6</v>
+        <v>16.7</v>
       </c>
       <c r="C15" t="n">
-        <v>22.186</v>
+        <v>22.167</v>
       </c>
     </row>
     <row r="16">
@@ -634,10 +634,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>82.59999999999999</v>
+        <v>83.7</v>
       </c>
       <c r="C16" t="n">
-        <v>6.524</v>
+        <v>6.582</v>
       </c>
     </row>
     <row r="17">
@@ -647,10 +647,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>32.5</v>
+        <v>35.2</v>
       </c>
       <c r="C17" t="n">
-        <v>9.718</v>
+        <v>9.044</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         <v>100</v>
       </c>
       <c r="C18" t="n">
-        <v>5.16</v>
+        <v>5.169</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>14.858</v>
+        <v>14.958</v>
       </c>
     </row>
     <row r="20">
@@ -702,7 +702,7 @@
         <v>100</v>
       </c>
       <c r="C21" t="n">
-        <v>13.743</v>
+        <v>13.446</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         <v>100</v>
       </c>
       <c r="C22" t="n">
-        <v>22.262</v>
+        <v>22.507</v>
       </c>
     </row>
     <row r="23">
@@ -767,7 +767,7 @@
         <v>100</v>
       </c>
       <c r="C26" t="n">
-        <v>15.794</v>
+        <v>15.823</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         <v>100</v>
       </c>
       <c r="C27" t="n">
-        <v>8.968</v>
+        <v>8.960000000000001</v>
       </c>
     </row>
     <row r="28">
@@ -790,10 +790,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>83.40000000000001</v>
+        <v>85.3</v>
       </c>
       <c r="C28" t="n">
-        <v>5.781</v>
+        <v>5.58</v>
       </c>
     </row>
     <row r="29">
@@ -803,10 +803,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>68.2</v>
+        <v>66.59999999999999</v>
       </c>
       <c r="C29" t="n">
-        <v>4.046</v>
+        <v>4.041</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         <v>0</v>
       </c>
       <c r="C30" t="n">
-        <v>15.999</v>
+        <v>16.479</v>
       </c>
     </row>
     <row r="31">
@@ -829,10 +829,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>18.1</v>
+        <v>19.6</v>
       </c>
       <c r="C31" t="n">
-        <v>27.57</v>
+        <v>27.12</v>
       </c>
     </row>
     <row r="32">
@@ -842,10 +842,10 @@
         </is>
       </c>
       <c r="B32" t="n">
-        <v>50</v>
+        <v>47.3</v>
       </c>
       <c r="C32" t="n">
-        <v>7.979</v>
+        <v>8.298999999999999</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         <v>100</v>
       </c>
       <c r="C33" t="n">
-        <v>4.934</v>
+        <v>5.021</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         <v>100</v>
       </c>
       <c r="C34" t="n">
-        <v>4.646</v>
+        <v>4.642</v>
       </c>
     </row>
     <row r="35">
@@ -881,10 +881,10 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>84</v>
+        <v>83.90000000000001</v>
       </c>
       <c r="C35" t="n">
-        <v>17.561</v>
+        <v>16.872</v>
       </c>
     </row>
     <row r="36">
@@ -894,10 +894,10 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>48.5</v>
+        <v>49.7</v>
       </c>
       <c r="C36" t="n">
-        <v>3.666</v>
+        <v>3.627</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,7 @@
         <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>17.68</v>
+        <v>17.92</v>
       </c>
     </row>
     <row r="38">
@@ -920,10 +920,10 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>84.5</v>
+        <v>80.8</v>
       </c>
       <c r="C38" t="n">
-        <v>7.438</v>
+        <v>7.204</v>
       </c>
     </row>
     <row r="39">
@@ -946,10 +946,10 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>49.5</v>
+        <v>49.6</v>
       </c>
       <c r="C40" t="n">
-        <v>8.489000000000001</v>
+        <v>8.792</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         <v>100</v>
       </c>
       <c r="C41" t="n">
-        <v>4.958</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -972,10 +972,10 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>50.2</v>
+        <v>49.3</v>
       </c>
       <c r="C42" t="n">
-        <v>3.84</v>
+        <v>3.862</v>
       </c>
     </row>
     <row r="43">
@@ -1011,10 +1011,10 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>17.5</v>
+        <v>17.4</v>
       </c>
       <c r="C45" t="n">
-        <v>13.554</v>
+        <v>13.545</v>
       </c>
     </row>
     <row r="46">
@@ -1024,10 +1024,10 @@
         </is>
       </c>
       <c r="B46" t="n">
-        <v>49.9</v>
+        <v>51.3</v>
       </c>
       <c r="C46" t="n">
-        <v>19.051</v>
+        <v>18.642</v>
       </c>
     </row>
     <row r="47">
@@ -1037,10 +1037,10 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>16.3</v>
+        <v>15.8</v>
       </c>
       <c r="C47" t="n">
-        <v>4.52</v>
+        <v>4.466</v>
       </c>
     </row>
   </sheetData>

</xml_diff>